<commit_message>
update Mobile check list
</commit_message>
<xml_diff>
--- a/Mobile_Testing.xlsx
+++ b/Mobile_Testing.xlsx
@@ -380,18 +380,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -403,6 +391,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,10 +703,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,10 +718,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,10 +787,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -928,10 +928,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1005,10 +1005,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="14"/>
+      <c r="B37" s="17"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -1056,10 +1056,10 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="15"/>
+      <c r="B43" s="18"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1107,10 +1107,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="14"/>
+      <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -1158,10 +1158,10 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="14"/>
+      <c r="B55" s="17"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -1191,10 +1191,10 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B59" s="15"/>
+      <c r="B59" s="18"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -1224,10 +1224,10 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B63" s="14"/>
+      <c r="B63" s="17"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -1266,10 +1266,10 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="14"/>
+      <c r="B68" s="17"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
@@ -1308,10 +1308,10 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="12"/>
+      <c r="B73" s="19"/>
       <c r="C73"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,18 +1429,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>